<commit_message>
added a new enum for auxiliary attacks, which show up in abilities menu but arent a status effect, ability, or mutation
</commit_message>
<xml_diff>
--- a/models/state_representations.xlsx
+++ b/models/state_representations.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbe28fe5e73b7d58/Code Projects/dcss-ai-wrapper/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="431" documentId="8_{D3E82A46-8DD3-4A77-9507-A268DA93A4BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6C6BB49E-FF06-4BAD-A6FC-8D81B2B8F0A9}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="8_{D3E82A46-8DD3-4A77-9507-A268DA93A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D1B1BA1-E74C-4092-B5EB-4F27374A35F3}"/>
   <bookViews>
-    <workbookView xWindow="25635" yWindow="4230" windowWidth="22905" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{E448CD2A-47DC-41F6-9276-34190ADF4EFE}"/>
+    <workbookView xWindow="18360" yWindow="3390" windowWidth="28170" windowHeight="15435" firstSheet="1" activeTab="2" xr2:uid="{E448CD2A-47DC-41F6-9276-34190ADF4EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Player Stats Vector" sheetId="1" r:id="rId1"/>
     <sheet name="PDDL Facts per API Call" sheetId="5" r:id="rId2"/>
-    <sheet name="Inventory Vector" sheetId="4" r:id="rId3"/>
-    <sheet name="status effects" sheetId="2" r:id="rId4"/>
-    <sheet name="mutations" sheetId="3" r:id="rId5"/>
-    <sheet name="terrain" sheetId="6" r:id="rId6"/>
-    <sheet name="monsters" sheetId="7" r:id="rId7"/>
+    <sheet name="auxiliaryattack" sheetId="8" r:id="rId3"/>
+    <sheet name="Inventory Vector" sheetId="4" r:id="rId4"/>
+    <sheet name="status effects" sheetId="2" r:id="rId5"/>
+    <sheet name="mutations" sheetId="3" r:id="rId6"/>
+    <sheet name="terrain" sheetId="6" r:id="rId7"/>
+    <sheet name="monsters" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="1182">
   <si>
     <t>Vector Index</t>
   </si>
@@ -3463,13 +3464,136 @@
   </si>
   <si>
     <t>spell_available_to_memorise</t>
+  </si>
+  <si>
+    <t>Offhand Punch</t>
+  </si>
+  <si>
+    <t>5 + UC/2</t>
+  </si>
+  <si>
+    <t>Wielding a shield prevents this, improves with Unarmed Combat skill</t>
+  </si>
+  <si>
+    <t>Offhand Punch w/ Claws</t>
+  </si>
+  <si>
+    <t>+1d3 × (Claws ranks)</t>
+  </si>
+  <si>
+    <t>Negated by Blade Hands or by wearing gloves</t>
+  </si>
+  <si>
+    <t>Offhand Punch w/ Blade Hands</t>
+  </si>
+  <si>
+    <t>Negates claws</t>
+  </si>
+  <si>
+    <t>Headbutt</t>
+  </si>
+  <si>
+    <t>5 + 3 × (Horns ranks)</t>
+  </si>
+  <si>
+    <t>Minotaurs occasionally counter enemy attacks that miss with this.</t>
+  </si>
+  <si>
+    <t>Peck</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Kick w/ Hooves</t>
+  </si>
+  <si>
+    <t>5 + (5/3) × (Hooves ranks)</t>
+  </si>
+  <si>
+    <t>Kick w/ Talons</t>
+  </si>
+  <si>
+    <t>6 + (Talons ranks)</t>
+  </si>
+  <si>
+    <t>Wearing boots negates this</t>
+  </si>
+  <si>
+    <t>Tail Slap</t>
+  </si>
+  <si>
+    <t>Grey draconians in deep water can push back their enemies</t>
+  </si>
+  <si>
+    <t>Tail Slap w/ Stinger</t>
+  </si>
+  <si>
+    <t>+1/3/5 (determined by Stinger ranks)</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>Venom</t>
+  </si>
+  <si>
+    <t>Bite w/ Fangs</t>
+  </si>
+  <si>
+    <t>2 × (Fangs ranks) +1 for every 5 STR beyond 10</t>
+  </si>
+  <si>
+    <t>Bloodless vampires have a vampiric bite</t>
+  </si>
+  <si>
+    <t>Bite w/ Acidic Bite</t>
+  </si>
+  <si>
+    <t>+ 2d4 acid splash</t>
+  </si>
+  <si>
+    <t>Corrosion</t>
+  </si>
+  <si>
+    <t>Bite w/ Anti-magic Bite</t>
+  </si>
+  <si>
+    <t>2 × (Fangs ranks) + XL/3</t>
+  </si>
+  <si>
+    <t>Anti-magic, Vine Stalker only</t>
+  </si>
+  <si>
+    <t>Pseudopods</t>
+  </si>
+  <si>
+    <t>4 × (Pseudopods rank)</t>
+  </si>
+  <si>
+    <t>Tentacle spike</t>
+  </si>
+  <si>
+    <t>5 + (Tentacle Spike rank)</t>
+  </si>
+  <si>
+    <t>Tentacle Slap</t>
+  </si>
+  <si>
+    <t>Octopodes' equivalent to the offhand punch</t>
+  </si>
+  <si>
+    <t>Tentacles (squeeze)</t>
+  </si>
+  <si>
+    <t>Constriction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3501,6 +3625,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3523,7 +3655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3538,6 +3670,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5914,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4F065C-A34E-4FF9-B6D7-F42747198C00}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6137,6 +6278,338 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D036E6-55A2-4721-8A86-2C26A6429BC1}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C1" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E1" t="str">
+        <f>UPPER(SUBSTITUTE(A1," ","_"))</f>
+        <v>OFFHAND_PUNCH</v>
+      </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE("(aux_attack ", LOWER(SUBSTITUTE(A1, " ", "_")), ")" )</f>
+        <v>(aux_attack offhand_punch)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E17" si="0">UPPER(SUBSTITUTE(A2," ","_"))</f>
+        <v>OFFHAND_PUNCH_W/_CLAWS</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>OFFHAND_PUNCH_W/_BLADE_HANDS</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>HEADBUTT</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B5" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>PECK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>KICK_W/_HOOVES</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>KICK_W/_TALONS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B8" s="7">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>TAIL_SLAP</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>TAIL_SLAP_W/_STINGER</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>BITE_W/_FANGS</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>BITE_W/_ACIDIC_BITE</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>BITE_W/_ANTI-MAGIC_BITE</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>PSEUDOPODS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>TENTACLE_SPIKE</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>TENTACLE_SLAP</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B16" s="7">
+        <v>12</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>TENTACLES_(SQUEEZE)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTRICTION</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71594451-649A-44E6-92D1-0C46CF4E6FB6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6148,12 +6621,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD5B03B-DEFB-4DC3-919E-A7A540AE896A}">
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8276,7 +8749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573E8D76-F880-4E8A-B7B5-A7A9ECA17AF4}">
   <dimension ref="A1:I64"/>
   <sheetViews>
@@ -9319,7 +9792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4342049E-AF89-4384-9A4C-686A2B259553}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -9538,7 +10011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D308D83-35AE-42C6-8A72-1778F955F227}">
   <dimension ref="A1:B732"/>
   <sheetViews>

</xml_diff>

<commit_message>
wrote constructor for spell class, refactored SpellType to SpellName
</commit_message>
<xml_diff>
--- a/models/state_representations.xlsx
+++ b/models/state_representations.xlsx
@@ -6282,7 +6282,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6459,7 @@
         <v>TAIL_SLAP_W/_STINGER</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1165</v>
       </c>

</xml_diff>